<commit_message>
re-design game, add gem
</commit_message>
<xml_diff>
--- a/map/map.xlsx
+++ b/map/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\game\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EA7393-5B3C-41F7-B55C-2BC1B53934AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCD8345-F023-4DEB-AD27-8A4ED06C8B87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DD570EC4-43C6-4FDC-B75A-A5E135922E27}"/>
   </bookViews>
@@ -30,10 +30,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33266D61-76E8-4505-9B4D-41D87BB1D00D}">
-  <dimension ref="A1:AD11"/>
+  <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AQ11" sqref="AQ11"/>
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,7 +404,7 @@
     <col min="22" max="22" width="3.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>0</v>
       </c>
@@ -451,50 +447,56 @@
       <c r="O1">
         <v>13</v>
       </c>
-      <c r="Q1">
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="R1">
         <v>0</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <v>1</v>
       </c>
-      <c r="S1">
+      <c r="T1">
         <v>2</v>
       </c>
-      <c r="T1">
+      <c r="U1">
         <v>3</v>
       </c>
-      <c r="U1">
+      <c r="V1">
         <v>4</v>
       </c>
-      <c r="V1">
+      <c r="W1">
         <v>5</v>
       </c>
-      <c r="W1">
+      <c r="X1">
         <v>6</v>
       </c>
-      <c r="X1">
+      <c r="Y1">
         <v>7</v>
       </c>
-      <c r="Y1">
+      <c r="Z1">
         <v>8</v>
       </c>
-      <c r="Z1">
+      <c r="AA1">
         <v>9</v>
       </c>
-      <c r="AA1">
+      <c r="AB1">
         <v>10</v>
       </c>
-      <c r="AB1">
+      <c r="AC1">
         <v>11</v>
       </c>
-      <c r="AC1">
+      <c r="AD1">
         <v>12</v>
       </c>
-      <c r="AD1">
+      <c r="AE1">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AF1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -512,10 +514,10 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2">
+      <c r="P2" s="1"/>
+      <c r="Q2">
         <v>0</v>
       </c>
-      <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -529,8 +531,10 @@
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -548,10 +552,10 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3">
+      <c r="P3" s="1"/>
+      <c r="Q3">
         <v>1</v>
       </c>
-      <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
@@ -561,12 +565,14 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -574,7 +580,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -584,10 +590,10 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4">
+      <c r="P4" s="1"/>
+      <c r="Q4">
         <v>2</v>
       </c>
-      <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -596,21 +602,23 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
-      <c r="Z4" s="2"/>
+      <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
+      <c r="AB4" s="2"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -620,10 +628,10 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5">
+      <c r="P5" s="1"/>
+      <c r="Q5">
         <v>3</v>
       </c>
-      <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -632,21 +640,23 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="2"/>
+      <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
+      <c r="AB5" s="2"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -656,13 +666,13 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6">
+      <c r="P6" s="1"/>
+      <c r="Q6">
         <v>4</v>
       </c>
-      <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
@@ -673,18 +683,20 @@
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -692,97 +704,103 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7">
+      <c r="P7" s="2"/>
+      <c r="Q7">
         <v>5</v>
       </c>
-      <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="2"/>
+      <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
+      <c r="U7" s="2"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
-      <c r="Z7" s="2"/>
+      <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
+      <c r="AB7" s="2"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8">
+      <c r="P8" s="1"/>
+      <c r="Q8">
         <v>6</v>
       </c>
-      <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="2"/>
+      <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
+      <c r="U8" s="2"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="2"/>
+      <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
+      <c r="AB8" s="2"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9">
+      <c r="P9" s="1"/>
+      <c r="Q9">
         <v>7</v>
       </c>
-      <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -800,10 +818,10 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10">
+      <c r="P10" s="1"/>
+      <c r="Q10">
         <v>8</v>
       </c>
-      <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -817,8 +835,10 @@
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -836,10 +856,10 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11">
+      <c r="P11" s="1"/>
+      <c r="Q11">
         <v>9</v>
       </c>
-      <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -853,6 +873,8 @@
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>